<commit_message>
Update named cells style
</commit_message>
<xml_diff>
--- a/test-data/test-data.xlsx
+++ b/test-data/test-data.xlsx
@@ -1,85 +1,75 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr codeName="ThisWorkbook"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\openpyxl-practice\test-data\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D39D6728-5A0B-4BB5-A681-009E83109479}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17200" yWindow="1500" windowWidth="10260" windowHeight="8940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView activeTab="1" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="8930" windowWidth="15140" xWindow="20890" yWindow="11590"/>
   </bookViews>
   <sheets>
-    <sheet name="Test1" sheetId="1" r:id="rId1"/>
+    <sheet name="Test1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Test2" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="TileMap">Test1!$B$3:$E$6</definedName>
+    <definedName name="TileMap2">Test2!$B$3:$E$6</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="162913" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="7">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Yu Gothic"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <name val="Yu Gothic"/>
+      <charset val="128"/>
+      <family val="3"/>
       <sz val="6"/>
-      <name val="Yu Gothic"/>
-      <family val="3"/>
-      <charset val="128"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="5" tint="0.79998168889431442"/>
       <name val="Yu Gothic"/>
       <family val="2"/>
+      <color theme="5" tint="0.7999816888943144"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="9" tint="0.79998168889431442"/>
       <name val="Yu Gothic"/>
       <family val="2"/>
+      <color theme="9" tint="0.7999816888943144"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="8" tint="0.79998168889431442"/>
       <name val="Yu Gothic"/>
       <family val="2"/>
+      <color theme="8" tint="0.7999816888943144"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="7"/>
       <name val="Yu Gothic"/>
       <family val="2"/>
+      <color theme="7"/>
+      <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <color rgb="00FF0000"/>
     </font>
   </fonts>
   <fills count="6">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -272,40 +262,100 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+  <cellXfs count="18">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="2" fillId="2" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="9" fillId="2" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="3" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="7" fillId="3" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="3" fillId="4" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="6" fillId="4" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="4" fillId="5" fontId="5" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="5" fillId="5" fontId="5" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="8" fillId="5" fontId="5" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="10" fillId="3" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="11" fillId="2" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="12" fillId="4" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="13" fillId="4" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="14" fillId="5" fontId="5" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="1" fillId="2" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="15" fillId="3" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="標準" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="標準" xfId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -571,76 +621,154 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr codeName="Sheet1"/>
-  <dimension ref="B2:E7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr codeName="Sheet1">
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="B3:E6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="18"/>
+  <sheetData>
+    <row customHeight="1" ht="18.5" r="2" thickBot="1"/>
+    <row customHeight="1" ht="18.5" r="3" thickTop="1">
+      <c r="B3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C3" s="10" t="n">
+        <v>2</v>
+      </c>
+      <c r="D3" s="5" t="n">
+        <v>3</v>
+      </c>
+      <c r="E3" s="7" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="18.5" r="4" thickBot="1">
+      <c r="B4" s="8" t="n">
+        <v>5</v>
+      </c>
+      <c r="C4" s="11" t="n">
+        <v>6</v>
+      </c>
+      <c r="D4" s="3" t="n">
+        <v>7</v>
+      </c>
+      <c r="E4" s="6" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="B5" s="13" t="n">
+        <v>9</v>
+      </c>
+      <c r="C5" s="14" t="n">
+        <v>10</v>
+      </c>
+      <c r="D5" s="15" t="n">
+        <v>11</v>
+      </c>
+      <c r="E5" s="16" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="18.5" r="6" thickBot="1">
+      <c r="B6" s="4" t="n">
+        <v>13</v>
+      </c>
+      <c r="C6" s="12" t="n">
+        <v>14</v>
+      </c>
+      <c r="D6" s="9" t="n">
+        <v>15</v>
+      </c>
+      <c r="E6" s="2" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="18.5" r="7" thickTop="1"/>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="B3:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B3" sqref="B3:E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="18"/>
   <sheetData>
-    <row r="2" spans="2:5" ht="18.5" thickBot="1"/>
-    <row r="3" spans="2:5" ht="18.5" thickTop="1">
-      <c r="B3" s="1">
-        <v>1</v>
-      </c>
-      <c r="C3" s="10">
-        <v>2</v>
-      </c>
-      <c r="D3" s="5">
-        <v>3</v>
-      </c>
-      <c r="E3" s="7">
-        <v>4</v>
+    <row r="3">
+      <c r="B3" s="17" t="n">
+        <v>7</v>
+      </c>
+      <c r="C3" s="17" t="n">
+        <v>8</v>
+      </c>
+      <c r="D3" s="17" t="n">
+        <v>9</v>
+      </c>
+      <c r="E3" s="17" t="n">
+        <v>10</v>
       </c>
     </row>
-    <row r="4" spans="2:5" ht="18.5" thickBot="1">
-      <c r="B4" s="8">
-        <v>5</v>
-      </c>
-      <c r="C4" s="11">
-        <v>6</v>
-      </c>
-      <c r="D4" s="3">
-        <v>7</v>
-      </c>
-      <c r="E4" s="6">
-        <v>8</v>
+    <row r="4">
+      <c r="B4" s="17" t="n">
+        <v>11</v>
+      </c>
+      <c r="C4" s="17" t="n">
+        <v>12</v>
+      </c>
+      <c r="D4" s="17" t="n">
+        <v>13</v>
+      </c>
+      <c r="E4" s="17" t="n">
+        <v>14</v>
       </c>
     </row>
-    <row r="5" spans="2:5">
-      <c r="B5" s="13">
-        <v>9</v>
-      </c>
-      <c r="C5" s="14">
-        <v>10</v>
-      </c>
-      <c r="D5" s="15">
-        <v>11</v>
-      </c>
-      <c r="E5" s="16">
-        <v>12</v>
+    <row r="5">
+      <c r="B5" s="17" t="n">
+        <v>15</v>
+      </c>
+      <c r="C5" s="17" t="n">
+        <v>16</v>
+      </c>
+      <c r="D5" s="17" t="n">
+        <v>17</v>
+      </c>
+      <c r="E5" s="17" t="n">
+        <v>18</v>
       </c>
     </row>
-    <row r="6" spans="2:5" ht="18.5" thickBot="1">
-      <c r="B6" s="4">
-        <v>13</v>
-      </c>
-      <c r="C6" s="12">
-        <v>14</v>
-      </c>
-      <c r="D6" s="9">
-        <v>15</v>
-      </c>
-      <c r="E6" s="2">
-        <v>16</v>
+    <row r="6">
+      <c r="B6" s="17" t="n">
+        <v>19</v>
+      </c>
+      <c r="C6" s="17" t="n">
+        <v>20</v>
+      </c>
+      <c r="D6" s="17" t="n">
+        <v>21</v>
+      </c>
+      <c r="E6" s="17" t="n">
+        <v>22</v>
       </c>
     </row>
-    <row r="7" spans="2:5" ht="18.5" thickTop="1"/>
   </sheetData>
-  <phoneticPr fontId="1"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup orientation="portrait" paperSize="9"/>
 </worksheet>
 </file>
</xml_diff>